<commit_message>
Mise à jour 11.03.2020
</commit_message>
<xml_diff>
--- a/Journal de bord.xlsx
+++ b/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Clion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planification du Projet </t>
+  </si>
+  <si>
+    <t>GitHub - https://github.com/TCamoes15/BatailleNavale-TiagoSantos</t>
   </si>
 </sst>
 </file>
@@ -146,17 +152,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -442,7 +448,7 @@
   <dimension ref="D2:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:P9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,44 +459,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D4" s="3">
@@ -507,7 +513,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="5"/>
@@ -631,15 +637,23 @@
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="3">
+        <v>43901</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -872,24 +886,42 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="L5:P5"/>
-    <mergeCell ref="L6:P6"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D2:P2"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="L18:P18"/>
+    <mergeCell ref="L19:P19"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="L12:P12"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="L15:P15"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="L22:P22"/>
+    <mergeCell ref="L23:P23"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="L25:P25"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="L21:P21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
@@ -906,42 +938,24 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="L22:P22"/>
-    <mergeCell ref="L23:P23"/>
-    <mergeCell ref="L24:P24"/>
-    <mergeCell ref="L25:P25"/>
-    <mergeCell ref="L20:P20"/>
-    <mergeCell ref="L21:P21"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="D2:P2"/>
-    <mergeCell ref="L16:P16"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="L18:P18"/>
-    <mergeCell ref="L19:P19"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="L12:P12"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="L14:P14"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="L15:P15"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="L6:P6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L4" r:id="rId1"/>

</xml_diff>